<commit_message>
still testing the action part and errors thrown with Custom fields
</commit_message>
<xml_diff>
--- a/data-manager/TestList.xlsx
+++ b/data-manager/TestList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,44 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Clodius, Rainer (BEB_HLI)</author>
+    <author>Rainer</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Test with comma values, too!
+          <t xml:space="preserve">works with ' : , " ∞
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rainer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+as those values will be handled as strings it is assumed that this will work (GUI does not support it yet)</t>
         </r>
       </text>
     </comment>
@@ -40,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="43">
   <si>
     <t>Testliste</t>
   </si>
@@ -175,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,7 +219,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -635,7 +666,10 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M7:N13"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,90 +726,90 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>11</v>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>11</v>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
+      <c r="F5" s="7">
+        <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>31</v>
@@ -797,20 +831,20 @@
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>31</v>
@@ -832,20 +866,20 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>11</v>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>31</v>
@@ -867,20 +901,20 @@
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>11</v>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>31</v>
@@ -902,20 +936,20 @@
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>11</v>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>31</v>
@@ -937,17 +971,17 @@
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>11</v>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>31</v>
@@ -958,8 +992,8 @@
       <c r="H10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>11</v>
+      <c r="I10" s="7">
+        <v>1</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>31</v>
@@ -972,17 +1006,17 @@
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>11</v>
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>31</v>
@@ -993,8 +1027,8 @@
       <c r="H11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>11</v>
+      <c r="I11" s="7">
+        <v>1</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>31</v>
@@ -1012,8 +1046,8 @@
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>11</v>
+      <c r="E12" s="7">
+        <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>31</v>
@@ -1030,8 +1064,8 @@
       <c r="J12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>11</v>
+      <c r="K12" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1043,8 +1077,8 @@
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
-        <v>11</v>
+      <c r="E13" s="7">
+        <v>1</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>31</v>
@@ -1061,8 +1095,8 @@
       <c r="J13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="7" t="s">
-        <v>11</v>
+      <c r="K13" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1074,8 +1108,8 @@
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>11</v>
+      <c r="E14" s="7">
+        <v>1</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>31</v>
@@ -1105,8 +1139,8 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
-        <v>11</v>
+      <c r="E15" s="7">
+        <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>31</v>
@@ -1136,8 +1170,8 @@
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>11</v>
+      <c r="E16" s="7">
+        <v>1</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>31</v>
@@ -1167,8 +1201,8 @@
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>11</v>
+      <c r="E17" s="7">
+        <v>1</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>31</v>
@@ -1198,8 +1232,8 @@
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
-        <v>11</v>
+      <c r="E18" s="7">
+        <v>1</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>31</v>
@@ -1216,8 +1250,8 @@
       <c r="J18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>11</v>
+      <c r="K18" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1229,8 +1263,8 @@
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
-        <v>11</v>
+      <c r="E19" s="7">
+        <v>1</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>31</v>
@@ -1247,8 +1281,8 @@
       <c r="J19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="7" t="s">
-        <v>11</v>
+      <c r="K19" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1260,8 +1294,8 @@
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
-        <v>11</v>
+      <c r="E20" s="7">
+        <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>31</v>
@@ -1278,8 +1312,8 @@
       <c r="J20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>11</v>
+      <c r="K20" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1291,8 +1325,8 @@
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="7" t="s">
-        <v>11</v>
+      <c r="E21" s="7">
+        <v>1</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>31</v>
@@ -1309,37 +1343,37 @@
       <c r="J21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K21" s="7" t="s">
-        <v>11</v>
+      <c r="K21" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>11</v>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>1</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8">
+        <v>1</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
still problems with calc modifier
</commit_message>
<xml_diff>
--- a/data-manager/TestList.xlsx
+++ b/data-manager/TestList.xlsx
@@ -59,12 +59,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="K28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rainer:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Add with {field} does not work</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="44">
   <si>
     <t>Testliste</t>
   </si>
@@ -193,6 +217,9 @@
   </si>
   <si>
     <t>failed</t>
+  </si>
+  <si>
+    <t>Add</t>
   </si>
 </sst>
 </file>
@@ -663,13 +690,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G1:H4"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,28 +1402,28 @@
       <c r="I22" s="8">
         <v>1</v>
       </c>
-      <c r="J22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>11</v>
+      <c r="J22" s="8">
+        <v>1</v>
+      </c>
+      <c r="K22" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>11</v>
+        <v>31</v>
+      </c>
+      <c r="E23" s="6">
+        <v>1</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>31</v>
@@ -1413,19 +1440,23 @@
       <c r="J23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="6" t="s">
-        <v>31</v>
+      <c r="K23" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="E24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1450,15 +1481,15 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
-        <v>11</v>
+      <c r="E25" s="6">
+        <v>1</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>31</v>
@@ -1475,21 +1506,21 @@
       <c r="J25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="6" t="s">
-        <v>11</v>
+      <c r="K25" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="6" t="s">
-        <v>11</v>
+      <c r="E26" s="6">
+        <v>1</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>31</v>
@@ -1506,100 +1537,131 @@
       <c r="J26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K26" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="K26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>31</v>
+      <c r="B28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J28" s="9">
+        <v>1</v>
+      </c>
+      <c r="K28" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="5">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B35" s="5">
         <v>-1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:K28">
+  <conditionalFormatting sqref="B3:K29">
     <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>$B$30</formula>
+      <formula>$B$31</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:K27">
+  <conditionalFormatting sqref="B3:K28">
     <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>$B$35</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
       <formula>$B$34</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
       <formula>$B$33</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
       <formula>$B$32</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
-      <formula>$B$31</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed - dmparser.equals returns case-sensitive comparison (not compatible to older DM versions) (issue 97) fixed - old value of book.Tags is empty when written to the log (issue 98) change - includes GUI r56
</commit_message>
<xml_diff>
--- a/data-manager/TestList.xlsx
+++ b/data-manager/TestList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="10035"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="13410" windowHeight="7515"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="44">
   <si>
     <t>Testliste</t>
   </si>
@@ -693,10 +693,10 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,17 +1448,17 @@
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>11</v>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
+        <v>1</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>31</v>
@@ -1475,8 +1475,8 @@
       <c r="J24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>11</v>
+      <c r="K24" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>